<commit_message>
Devops i dorada gresaka
</commit_message>
<xml_diff>
--- a/report/SONARQUBE_REPORT_sr.xlsx
+++ b/report/SONARQUBE_REPORT_sr.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
   <si>
     <t xml:space="preserve">Sample SonarQube Report</t>
   </si>
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Datum</t>
   </si>
   <si>
-    <t xml:space="preserve">28.2.2024.</t>
+    <t xml:space="preserve">20.3.2025.</t>
   </si>
   <si>
     <t xml:space="preserve">#</t>
@@ -52,10 +52,43 @@
     <t xml:space="preserve">Rezultat</t>
   </si>
   <si>
+    <t xml:space="preserve">Komentar</t>
+  </si>
+  <si>
     <t xml:space="preserve">SQL injection</t>
   </si>
   <si>
     <t xml:space="preserve">true positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">searchTerm unosi korisnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false positive</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bookId je int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">roleId je int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personId je int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personUpdate.getLastName() i personUpdate.getId() su int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rating.getUserId() i rating.getBookId() su int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">userId je int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username unosi korisnik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">username I password unosi korisnik</t>
   </si>
 </sst>
 </file>
@@ -156,13 +189,17 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -173,7 +210,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -195,7 +232,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -221,7 +258,21 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006100"/>
         </patternFill>
       </fill>
     </dxf>
@@ -327,9 +378,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2880</xdr:colOff>
+      <xdr:colOff>2520</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>20160</xdr:rowOff>
+      <xdr:rowOff>19800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -343,7 +394,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="905040"/>
-          <a:ext cx="7629840" cy="2066760"/>
+          <a:ext cx="7629480" cy="2066400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -364,9 +415,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>2103840</xdr:rowOff>
+      <xdr:rowOff>2103480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -380,7 +431,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2848680" y="2979720"/>
-          <a:ext cx="7626960" cy="2075760"/>
+          <a:ext cx="7626600" cy="2075400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -401,9 +452,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4377600</xdr:colOff>
+      <xdr:colOff>4377240</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>2055960</xdr:rowOff>
+      <xdr:rowOff>2055600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -417,7 +468,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="5074200"/>
-          <a:ext cx="4377600" cy="2055960"/>
+          <a:ext cx="4377240" cy="2055600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -438,9 +489,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5272200</xdr:colOff>
+      <xdr:colOff>5271840</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>2476080</xdr:rowOff>
+      <xdr:rowOff>2475720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -454,7 +505,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="7149600"/>
-          <a:ext cx="5272200" cy="2476080"/>
+          <a:ext cx="5271840" cy="2475720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -475,9 +526,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5272200</xdr:colOff>
+      <xdr:colOff>5271840</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -491,7 +542,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="12115080"/>
-          <a:ext cx="5272200" cy="2477160"/>
+          <a:ext cx="5271840" cy="2476800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -512,9 +563,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5272200</xdr:colOff>
+      <xdr:colOff>5271840</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>13320</xdr:rowOff>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -528,7 +579,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="9651240"/>
-          <a:ext cx="5272200" cy="2477160"/>
+          <a:ext cx="5271840" cy="2476800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -549,9 +600,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>5272200</xdr:colOff>
+      <xdr:colOff>5271840</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>2477160</xdr:rowOff>
+      <xdr:rowOff>2476800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -565,7 +616,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="27201960"/>
-          <a:ext cx="5272200" cy="2477160"/>
+          <a:ext cx="5271840" cy="2476800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -586,9 +637,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6875640</xdr:colOff>
+      <xdr:colOff>6875280</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:rowOff>26640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -602,7 +653,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="39824640"/>
-          <a:ext cx="6875640" cy="2092680"/>
+          <a:ext cx="6875280" cy="2092320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -623,9 +674,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7617240</xdr:colOff>
+      <xdr:colOff>7616880</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>1407240</xdr:rowOff>
+      <xdr:rowOff>1406880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -639,7 +690,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="41890320"/>
-          <a:ext cx="7617240" cy="1407240"/>
+          <a:ext cx="7616880" cy="1406880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -660,9 +711,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4642560</xdr:colOff>
+      <xdr:colOff>4642200</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>6480</xdr:rowOff>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -676,7 +727,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="43301880"/>
-          <a:ext cx="4642560" cy="1560240"/>
+          <a:ext cx="4642200" cy="1559880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -697,9 +748,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7594200</xdr:colOff>
+      <xdr:colOff>7593840</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>1553760</xdr:rowOff>
+      <xdr:rowOff>1553400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -713,7 +764,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2809440" y="37304640"/>
-          <a:ext cx="7613640" cy="1524960"/>
+          <a:ext cx="7613280" cy="1524600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -734,9 +785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7584120</xdr:colOff>
+      <xdr:colOff>7583760</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>1665000</xdr:rowOff>
+      <xdr:rowOff>1664640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -750,7 +801,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="24595920"/>
-          <a:ext cx="7584120" cy="1665000"/>
+          <a:ext cx="7583760" cy="1664640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -771,9 +822,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7577640</xdr:colOff>
+      <xdr:colOff>7577280</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>1484280</xdr:rowOff>
+      <xdr:rowOff>1483920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -787,7 +838,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="22094280"/>
-          <a:ext cx="7577640" cy="1484280"/>
+          <a:ext cx="7577280" cy="1483920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -808,9 +859,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>16560</xdr:colOff>
+      <xdr:colOff>16200</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>1845720</xdr:rowOff>
+      <xdr:rowOff>1845360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -824,7 +875,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="19563840"/>
-          <a:ext cx="7643520" cy="1845720"/>
+          <a:ext cx="7643160" cy="1845360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -845,9 +896,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7584120</xdr:colOff>
+      <xdr:colOff>7583760</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>1950480</xdr:rowOff>
+      <xdr:rowOff>1950120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -861,7 +912,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="17052120"/>
-          <a:ext cx="7584120" cy="1950480"/>
+          <a:ext cx="7583760" cy="1950120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -882,9 +933,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7576560</xdr:colOff>
+      <xdr:colOff>7576200</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1883880</xdr:rowOff>
+      <xdr:rowOff>1883520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -898,7 +949,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="14578920"/>
-          <a:ext cx="7576560" cy="1883880"/>
+          <a:ext cx="7576200" cy="1883520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -919,9 +970,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7538760</xdr:colOff>
+      <xdr:colOff>7538400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>1874520</xdr:rowOff>
+      <xdr:rowOff>1874160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -935,7 +986,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="34707960"/>
-          <a:ext cx="7538760" cy="1874520"/>
+          <a:ext cx="7538400" cy="1874160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -956,9 +1007,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7588440</xdr:colOff>
+      <xdr:colOff>7588080</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>2112120</xdr:rowOff>
+      <xdr:rowOff>2111760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -972,7 +1023,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="32215320"/>
-          <a:ext cx="7588440" cy="2112120"/>
+          <a:ext cx="7588080" cy="2111760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -993,9 +1044,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>20520</xdr:colOff>
+      <xdr:colOff>20160</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>1721880</xdr:rowOff>
+      <xdr:rowOff>1721520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1009,7 +1060,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="2828880" y="29713680"/>
-          <a:ext cx="7647480" cy="1721880"/>
+          <a:ext cx="7647120" cy="1721520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1035,9 +1086,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>574920</xdr:colOff>
+      <xdr:colOff>574560</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>50040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1051,7 +1102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="765360" y="200160"/>
-          <a:ext cx="7397640" cy="5279400"/>
+          <a:ext cx="7397280" cy="5279040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1083,232 +1134,293 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="85.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="85.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="13.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33.19"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>8</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="161.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5" t="n">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>10</v>
+      <c r="D6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="167.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="5" t="n">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
+      <c r="D7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="163.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4" t="s">
-        <v>10</v>
+      <c r="B8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="197" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>10</v>
+      <c r="B9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="194" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>10</v>
+      <c r="B10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="194" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>10</v>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="194.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>10</v>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="197.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>10</v>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="199.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>10</v>
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="197" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>10</v>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="205.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>10</v>
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="197.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B17" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>10</v>
+      <c r="B17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="197" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>10</v>
+      <c r="B18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="196.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>10</v>
+      <c r="B19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="202.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>10</v>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="200.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>10</v>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="162.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>10</v>
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="111.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>10</v>
+      <c r="B23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="122.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>10</v>
+      <c r="B24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D6:D24">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
       <formula>"false positive"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
       <formula>"true positive"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>